<commit_message>
POM with Data Driver
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\IdeaProjects\MyNewFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4856D460-F938-4DE5-9A7F-A08937E9FB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9200F07-3382-4522-ADB1-A8F4AD84CA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{C6EC2BE6-2F26-445B-950A-0AF3181E050B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>123456789</t>
   </si>
@@ -443,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4985C074-733C-4E60-B753-4169B92C5FB2}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="214" zoomScaleNormal="214" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B16" sqref="B16:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,6 +583,26 @@
         <v>16</v>
       </c>
     </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>